<commit_message>
Update Leader Note up to 17
</commit_message>
<xml_diff>
--- a/Leader's note.xlsx
+++ b/Leader's note.xlsx
@@ -5,48 +5,48 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wvi365-my.sharepoint.com/personal/arkar_linn_visionfund_org/Documents/Desktop/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/05d227db91bf3aa2/GitHub/tis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{BC9FD343-DC0A-4AC8-A18C-1F69C7E27C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8EC9015-32FD-4318-B123-D59638C6ACDC}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{BC9FD343-DC0A-4AC8-A18C-1F69C7E27C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C1C37C1-D69E-46D1-ADE2-D4776AF41F15}"/>
   <bookViews>
-    <workbookView xWindow="30105" yWindow="-3525" windowWidth="19755" windowHeight="20985" tabRatio="847" firstSheet="23" activeTab="33" xr2:uid="{926027B3-CA24-4164-B444-5B6AFF725907}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="955" firstSheet="9" activeTab="16" xr2:uid="{926027B3-CA24-4164-B444-5B6AFF725907}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
-    <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
-    <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
-    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
-    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
-    <sheet name="Sheet16" sheetId="16" r:id="rId16"/>
-    <sheet name="Sheet17" sheetId="17" r:id="rId17"/>
-    <sheet name="Sheet18" sheetId="18" r:id="rId18"/>
-    <sheet name="Sheet19" sheetId="19" r:id="rId19"/>
-    <sheet name="Sheet20" sheetId="20" r:id="rId20"/>
-    <sheet name="Sheet21" sheetId="21" r:id="rId21"/>
-    <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
-    <sheet name="Sheet23" sheetId="23" r:id="rId23"/>
-    <sheet name="Sheet24" sheetId="24" r:id="rId24"/>
-    <sheet name="Sheet25" sheetId="25" r:id="rId25"/>
-    <sheet name="Sheet26" sheetId="26" r:id="rId26"/>
-    <sheet name="Sheet27" sheetId="27" r:id="rId27"/>
-    <sheet name="Sheet28" sheetId="28" r:id="rId28"/>
-    <sheet name="Sheet29" sheetId="29" r:id="rId29"/>
-    <sheet name="Sheet30" sheetId="30" r:id="rId30"/>
-    <sheet name="Sheet31" sheetId="31" r:id="rId31"/>
-    <sheet name="Sheet32" sheetId="32" r:id="rId32"/>
-    <sheet name="Sheet33" sheetId="33" r:id="rId33"/>
-    <sheet name="Sheet34" sheetId="34" r:id="rId34"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="3" sheetId="3" r:id="rId3"/>
+    <sheet name="4" sheetId="4" r:id="rId4"/>
+    <sheet name="5" sheetId="5" r:id="rId5"/>
+    <sheet name="6" sheetId="6" r:id="rId6"/>
+    <sheet name="7" sheetId="7" r:id="rId7"/>
+    <sheet name="8" sheetId="8" r:id="rId8"/>
+    <sheet name="9" sheetId="9" r:id="rId9"/>
+    <sheet name="10" sheetId="10" r:id="rId10"/>
+    <sheet name="11" sheetId="11" r:id="rId11"/>
+    <sheet name="12" sheetId="12" r:id="rId12"/>
+    <sheet name="13" sheetId="13" r:id="rId13"/>
+    <sheet name="14" sheetId="14" r:id="rId14"/>
+    <sheet name="15" sheetId="15" r:id="rId15"/>
+    <sheet name="16" sheetId="16" r:id="rId16"/>
+    <sheet name="17" sheetId="17" r:id="rId17"/>
+    <sheet name="18" sheetId="18" r:id="rId18"/>
+    <sheet name="19" sheetId="19" r:id="rId19"/>
+    <sheet name="20" sheetId="20" r:id="rId20"/>
+    <sheet name="21" sheetId="21" r:id="rId21"/>
+    <sheet name="22" sheetId="22" r:id="rId22"/>
+    <sheet name="23" sheetId="23" r:id="rId23"/>
+    <sheet name="24" sheetId="24" r:id="rId24"/>
+    <sheet name="25" sheetId="25" r:id="rId25"/>
+    <sheet name="26" sheetId="26" r:id="rId26"/>
+    <sheet name="27" sheetId="27" r:id="rId27"/>
+    <sheet name="28" sheetId="28" r:id="rId28"/>
+    <sheet name="29" sheetId="29" r:id="rId29"/>
+    <sheet name="30" sheetId="30" r:id="rId30"/>
+    <sheet name="31" sheetId="31" r:id="rId31"/>
+    <sheet name="32" sheetId="32" r:id="rId32"/>
+    <sheet name="33" sheetId="33" r:id="rId33"/>
+    <sheet name="34" sheetId="34" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>မင်္ဂလာပါ... ကျွန်တော် Arkar ပါ။ 👋
 Microfinance လုပ်ငန်းခွင်ထဲမှာ ကျွန်တော် ၁၀ နှစ်ကျော် ဖြတ်သန်းခဲ့ပါတယ်။ ဒီခရီးလမ်းက လွယ်ကူခဲ့တာတော့ မဟုတ်ပါဘူး။
@@ -876,6 +876,37 @@
 👇 Start Learning Here: 👇
 (Website Link in Comment Section)
 #Excel #business #insight #Solutions #leadership </t>
+  </si>
+  <si>
+    <t>Excel လား? Power BI လား? ဘယ်အချိန်မှာ ဘာကိုသုံးမလဲ? ⚔️📊
+"ကိုအာကာ... Power BI ပေါ်လာပြီဆိုတော့ Excel က ခေတ်ကုန်သွားပြီလား?"
+"Report တွေလုပ်ဖို့ ဘယ်ဟာကို အဓိက လေ့လာသင့်လဲ?"
+ဒီမေးခွန်းတွေက Data လောကထဲ ဝင်လာသူတိုင်း မေးလေ့ရှိတဲ့ မေးခွန်းတွေပါ။
+ကျနော့်အဖြေကတော့ - "သူတို့နှစ်ခုက ပြိုင်ဘက်တွေ မဟုတ်ပါဘူး၊ မိတ်ဖက် (Partner) တွေပါ" ဆိုတာပါပဲ။
+ဘယ်အချိန်မှာ ဘာကိုသုံးမလဲဆိုတာ "ရည်ရွယ်ချက် (Purpose)" ပေါ်မှာ မူတည်ပါတယ်။
+၁။ Excel ကို ဘယ်အချိန်သုံးမလဲ? (The Flexible Workspace) 📗
+Excel ဆိုတာ Data တွေရဲ့ "မီးဖိုချောင်" လိုပါပဲ။
+✅ Data Entry &amp; Cleaning: Data တွေကို ပြင်ချင်၊ ဖြည့်ချင်၊ စစ်ဆေးချင်တဲ့အခါ Excel က အကောင်းဆုံးပါ။
+✅ Ad-hoc Analysis: ချက်ချင်း လက်တန်းတွက်ချက်ရမယ့် ကိစ္စတွေ၊ ရှုပ်ထွေးတဲ့ Financial Model တွေ တွက်တဲ့အခါ Excel က King ပါ။
+✅ Small Data: Data ပမာဏ မများဘူး၊ မြန်မြန်ဆန်ဆန် အဖြေလိုချင်ရင် Excel ကို ရွေးပါ။
+၂။ Power BI ကို ဘယ်အချိန်သုံးမလဲ? (The Powerful Display) 📊
+Power BI ဆိုတာကတော့ ချက်ပြုတ်ပြီးသား ဟင်းပွဲတွေကို ခင်းကျင်းပြသတဲ့ "ထမင်းစားပွဲ" နဲ့ တူပါတယ်။
+✅ Automation: လစဉ် Report တွေကို ထပ်ခါထပ်ခါ လုပ်စရာမလိုဘဲ Auto Refresh လုပ်ချင်ရင် Power BI ကို သုံးပါ။
+✅ Large Data: Excel က Row ၁ သန်းကျော်ရင် လေးလံသွားပေမယ့်၊ Power BI က Row သန်းချီကို ပေါ့ပါးစွာ ကိုင်တွယ်နိုင်ပါတယ်။
+✅ Interactive Dashboard: Boss တွေကို Click နှိပ်ပြီး ကိုယ်တိုင်ကြည့်လို့ရတဲ့ Dashboard မျိုး ပေးချင်ရင် Power BI က အကောင်းဆုံးပါ။
+✅ Security: ကိုယ့် Data ကို သူများဝင်မပြင်စေချင်ရင် (Read-only) အနေနဲ့ Share ဖို့ Power BI က စိတ်ချရပါတယ်။
+Summary (သုံးသပ်ချက်)
+မိတ်ဆွေက Data ကို "မွေးထုတ်ပြီး ပြုပြင်မယ့်သူ" ဆိုရင် Excel ကို ပိုင်နိုင်အောင် လုပ်ပါ။
+မိတ်ဆွေက Data ကို "ဆုံးဖြတ်ချက်ချဖို့ တင်ပြမယ့်သူ" ဆိုရင် Power BI ကို ထပ်ဖြည့်ပါ။
+Senior Level ရောက်လာလေ... ဒီလက်နက်နှစ်ခုလုံးကို ဘယ်အချိန်မှာ ထုတ်သုံးရမလဲဆိုတာ သိလေပါပဲ။ တူ (Hammer) နဲ့ထုရမယ့်နေရာမှာ ဝက်အူလှည့် (Screwdriver) သွားသုံးနေရင် အချိန်ကုန်ပြီး လူပန်းပါလိမ့်မယ်။
+ကဲ... မိတ်ဆွေကရော လက်ရှိမှာ ဘယ် Tool ကို ပိုအားသန်နေလဲ? Comment မှာ ဆွေးနွေးသွားလို့ ရပါတယ်ဗျာ။ 👇
+💡 Call to Action
+✅ Foundation (Excel):
+Data ကို စိတ်ကြိုက်ကစားဖို့ Excel Logic တွေကို အရင်ပိုင်နိုင်ချင်ရင် "Excel for Business Management" အတန်းရှိပါတယ်။
+👉 Register Here: [Google Form Link in comment]
+🚀 Visualization (Power BI):
+Excel နဲ့တင်မကတော့ဘဲ Report တွေကို Automation လုပ်ပြီး Dashboard အမိုက်စားတွေ ဆွဲချင်ရင်တော့ "Power BI Basic to Master (Jan Intake)" အတွက် လူစာရင်း စပေးသွင်းလို့ ရပါပြီ။ (Seats Limited!)
+#TheInsightsSolution #DataInsightsWithArkar #LeadersNote #Day17 #ExcelVsPowerBI #ToolSelection #DataAnalytics</t>
   </si>
 </sst>
 </file>
@@ -1277,11 +1308,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D5DE28-4C17-4DD7-BB74-FD64E0044119}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="154.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1297,11 +1331,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490AB32B-6769-4C0E-BEEA-01AF3319056B}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="190" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1315,13 +1352,19 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2CB876-9987-4C4C-859E-EEF38772F081}">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="159.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1335,16 +1378,25 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E25A69-3CCE-4042-A2E5-474D1730DD71}">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3:BN3"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="66" max="66" width="95.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:66" ht="198.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BN3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1355,13 +1407,19 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C872A52-1806-4BE3-AD77-55C527F627C4}">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="160.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1375,15 +1433,18 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2FEEE8-677F-4118-B2EF-77FE274ECB1F}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="112.54296875" customWidth="1"/>
+    <col min="3" max="3" width="149" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="409.5" x14ac:dyDescent="0.35">
@@ -1398,13 +1459,19 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52F40ADA-AF60-4B19-B1F7-A7F4B9A21D2F}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="204" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="3:3" ht="409.5" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
@@ -1418,17 +1485,23 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8536F09A-AE82-4D62-B95B-6605627D469F}">
-  <dimension ref="C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="3" spans="3:3" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="C3" s="1" t="s">
-        <v>15</v>
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="136.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:3" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="C2" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1514,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1464,7 +1537,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1507,7 +1580,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1527,7 +1600,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1547,7 +1620,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1567,7 +1640,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H15:H43"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1587,7 +1660,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1607,7 +1680,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1627,7 +1700,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1647,7 +1720,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1667,7 +1740,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1687,7 +1760,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1730,7 +1803,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1750,7 +1823,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1770,7 +1843,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1790,7 +1863,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1809,11 +1882,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829A3F37-4F4E-4564-9D05-C4AB6D014335}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="36.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1852,13 +1928,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB727769-C987-4F37-AF4D-44AF2BDE4453}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="182.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" ht="391.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1872,11 +1951,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB297D9-3B78-4A28-9CB9-57355CDFB6C2}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="191.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1892,11 +1974,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BE83D8-1DC7-49E0-A63D-F4745BB49B54}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="201.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1912,11 +1997,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930B20B1-4A68-4EC0-B4B0-707AEA232E42}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="166.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
@@ -1932,11 +2020,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC71656-FBBB-44D8-B490-1930B82C9459}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="172.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="2:2" ht="409.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">

</xml_diff>